<commit_message>
few changes and added IretryMechanism and IAnnotationTransformer
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -163,58 +163,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -600,7 +549,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="M10" sqref="L10:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>